<commit_message>
Changed the project documentation from word typesetting to LaTeX. Finished off the feasibility study and made some changes to different sections. Also added information pertaining to the development of blockchain technology in the algorithms section.
</commit_message>
<xml_diff>
--- a/Project Documentation/GANTT Chart for Major.xlsx
+++ b/Project Documentation/GANTT Chart for Major.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Alex\converge\Project Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{204CC944-DD33-4366-87E7-B7E44E1DF4A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1048F73-C38D-4A87-B8B1-36477939D12D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-103" yWindow="-103" windowWidth="22149" windowHeight="11949" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -17,7 +17,7 @@
   </sheets>
   <definedNames>
     <definedName name="prevWBS" localSheetId="0">GanttChart!$A1048576</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">GanttChart!$A$1:$BN$30</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">GanttChart!$A$1:$BN$31</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="0">GanttChart!$4:$7</definedName>
     <definedName name="valuevx">42.314159</definedName>
     <definedName name="vertex42_copyright" hidden="1">"© 2006-2018 Vertex42 LLC"</definedName>
@@ -426,7 +426,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="38">
   <si>
     <t>WBS</t>
   </si>
@@ -537,6 +537,9 @@
   </si>
   <si>
     <t>Meeting with CFO Mr Fong for continuous communication surrounding project timeline.</t>
+  </si>
+  <si>
+    <t>Smart Contracts that better facilitate the transfer of assets between companies. Also enable companies to create their own automated contracts for procurement and other financial processes.</t>
   </si>
 </sst>
 </file>
@@ -1259,7 +1262,7 @@
     <xf numFmtId="0" fontId="24" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="82">
+  <cellXfs count="87">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyProtection="1"/>
     <xf numFmtId="0" fontId="0" fillId="20" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyProtection="1"/>
@@ -1453,24 +1456,6 @@
     <xf numFmtId="169" fontId="30" fillId="21" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="36" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="36" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="36" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="33" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="33" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="33" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="43" fillId="0" borderId="0" xfId="34" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -1478,9 +1463,42 @@
       <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="36" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="36" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="36" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="168" fontId="33" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
       <protection locked="0"/>
+    </xf>
+    <xf numFmtId="167" fontId="33" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="33" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="33" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="35" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="169" fontId="35" fillId="22" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="169" fontId="35" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="35" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="38" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="44">
@@ -2085,11 +2103,11 @@
   <sheetPr codeName="Sheet8">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:CB31"/>
+  <dimension ref="A1:CB32"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="25" zoomScaleNormal="25" workbookViewId="0">
-      <pane ySplit="7" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B22" sqref="B22"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <pane ySplit="7" topLeftCell="A24" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G31" sqref="G31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.07421875" defaultRowHeight="12.45" x14ac:dyDescent="0.3"/>
@@ -2118,27 +2136,27 @@
       <c r="E1" s="10"/>
       <c r="F1" s="10"/>
       <c r="I1" s="64"/>
-      <c r="K1" s="79"/>
-      <c r="L1" s="79"/>
-      <c r="M1" s="79"/>
-      <c r="N1" s="79"/>
-      <c r="O1" s="79"/>
-      <c r="P1" s="79"/>
-      <c r="Q1" s="79"/>
-      <c r="R1" s="79"/>
-      <c r="S1" s="79"/>
-      <c r="T1" s="79"/>
-      <c r="U1" s="79"/>
-      <c r="V1" s="79"/>
-      <c r="W1" s="79"/>
-      <c r="X1" s="79"/>
-      <c r="Y1" s="79"/>
-      <c r="Z1" s="79"/>
-      <c r="AA1" s="79"/>
-      <c r="AB1" s="79"/>
-      <c r="AC1" s="79"/>
-      <c r="AD1" s="79"/>
-      <c r="AE1" s="79"/>
+      <c r="K1" s="73"/>
+      <c r="L1" s="73"/>
+      <c r="M1" s="73"/>
+      <c r="N1" s="73"/>
+      <c r="O1" s="73"/>
+      <c r="P1" s="73"/>
+      <c r="Q1" s="73"/>
+      <c r="R1" s="73"/>
+      <c r="S1" s="73"/>
+      <c r="T1" s="73"/>
+      <c r="U1" s="73"/>
+      <c r="V1" s="73"/>
+      <c r="W1" s="73"/>
+      <c r="X1" s="73"/>
+      <c r="Y1" s="73"/>
+      <c r="Z1" s="73"/>
+      <c r="AA1" s="73"/>
+      <c r="AB1" s="73"/>
+      <c r="AC1" s="73"/>
+      <c r="AD1" s="73"/>
+      <c r="AE1" s="73"/>
     </row>
     <row r="2" spans="1:80" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="67" t="s">
@@ -2184,11 +2202,11 @@
       <c r="B4" s="49" t="s">
         <v>9</v>
       </c>
-      <c r="C4" s="81">
+      <c r="C4" s="78">
         <v>44661</v>
       </c>
-      <c r="D4" s="81"/>
-      <c r="E4" s="81"/>
+      <c r="D4" s="78"/>
+      <c r="E4" s="78"/>
       <c r="F4" s="46"/>
       <c r="G4" s="49" t="s">
         <v>8</v>
@@ -2198,222 +2216,222 @@
       </c>
       <c r="I4" s="47"/>
       <c r="J4" s="13"/>
-      <c r="K4" s="73" t="str">
+      <c r="K4" s="75" t="str">
         <f>"Week "&amp;(K6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 1</v>
       </c>
-      <c r="L4" s="74"/>
-      <c r="M4" s="74"/>
-      <c r="N4" s="74"/>
-      <c r="O4" s="74"/>
-      <c r="P4" s="74"/>
-      <c r="Q4" s="75"/>
-      <c r="R4" s="73" t="str">
+      <c r="L4" s="76"/>
+      <c r="M4" s="76"/>
+      <c r="N4" s="76"/>
+      <c r="O4" s="76"/>
+      <c r="P4" s="76"/>
+      <c r="Q4" s="77"/>
+      <c r="R4" s="75" t="str">
         <f>"Week "&amp;(R6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 2</v>
       </c>
-      <c r="S4" s="74"/>
-      <c r="T4" s="74"/>
-      <c r="U4" s="74"/>
-      <c r="V4" s="74"/>
-      <c r="W4" s="74"/>
-      <c r="X4" s="75"/>
-      <c r="Y4" s="73" t="str">
+      <c r="S4" s="76"/>
+      <c r="T4" s="76"/>
+      <c r="U4" s="76"/>
+      <c r="V4" s="76"/>
+      <c r="W4" s="76"/>
+      <c r="X4" s="77"/>
+      <c r="Y4" s="75" t="str">
         <f>"Week "&amp;(Y6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 3</v>
       </c>
-      <c r="Z4" s="74"/>
-      <c r="AA4" s="74"/>
-      <c r="AB4" s="74"/>
-      <c r="AC4" s="74"/>
-      <c r="AD4" s="74"/>
-      <c r="AE4" s="75"/>
-      <c r="AF4" s="73" t="str">
+      <c r="Z4" s="76"/>
+      <c r="AA4" s="76"/>
+      <c r="AB4" s="76"/>
+      <c r="AC4" s="76"/>
+      <c r="AD4" s="76"/>
+      <c r="AE4" s="77"/>
+      <c r="AF4" s="75" t="str">
         <f>"Week "&amp;(AF6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 4</v>
       </c>
-      <c r="AG4" s="74"/>
-      <c r="AH4" s="74"/>
-      <c r="AI4" s="74"/>
-      <c r="AJ4" s="74"/>
-      <c r="AK4" s="74"/>
-      <c r="AL4" s="75"/>
-      <c r="AM4" s="73" t="str">
+      <c r="AG4" s="76"/>
+      <c r="AH4" s="76"/>
+      <c r="AI4" s="76"/>
+      <c r="AJ4" s="76"/>
+      <c r="AK4" s="76"/>
+      <c r="AL4" s="77"/>
+      <c r="AM4" s="75" t="str">
         <f>"Week "&amp;(AM6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 5</v>
       </c>
-      <c r="AN4" s="74"/>
-      <c r="AO4" s="74"/>
-      <c r="AP4" s="74"/>
-      <c r="AQ4" s="74"/>
-      <c r="AR4" s="74"/>
-      <c r="AS4" s="75"/>
-      <c r="AT4" s="73" t="str">
+      <c r="AN4" s="76"/>
+      <c r="AO4" s="76"/>
+      <c r="AP4" s="76"/>
+      <c r="AQ4" s="76"/>
+      <c r="AR4" s="76"/>
+      <c r="AS4" s="77"/>
+      <c r="AT4" s="75" t="str">
         <f>"Week "&amp;(AT6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 6</v>
       </c>
-      <c r="AU4" s="74"/>
-      <c r="AV4" s="74"/>
-      <c r="AW4" s="74"/>
-      <c r="AX4" s="74"/>
-      <c r="AY4" s="74"/>
-      <c r="AZ4" s="75"/>
-      <c r="BA4" s="73" t="str">
+      <c r="AU4" s="76"/>
+      <c r="AV4" s="76"/>
+      <c r="AW4" s="76"/>
+      <c r="AX4" s="76"/>
+      <c r="AY4" s="76"/>
+      <c r="AZ4" s="77"/>
+      <c r="BA4" s="75" t="str">
         <f>"Week "&amp;(BA6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 7</v>
       </c>
-      <c r="BB4" s="74"/>
-      <c r="BC4" s="74"/>
-      <c r="BD4" s="74"/>
-      <c r="BE4" s="74"/>
-      <c r="BF4" s="74"/>
-      <c r="BG4" s="75"/>
-      <c r="BH4" s="73" t="str">
+      <c r="BB4" s="76"/>
+      <c r="BC4" s="76"/>
+      <c r="BD4" s="76"/>
+      <c r="BE4" s="76"/>
+      <c r="BF4" s="76"/>
+      <c r="BG4" s="77"/>
+      <c r="BH4" s="75" t="str">
         <f>"Week "&amp;(BH6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 8</v>
       </c>
-      <c r="BI4" s="74"/>
-      <c r="BJ4" s="74"/>
-      <c r="BK4" s="74"/>
-      <c r="BL4" s="74"/>
-      <c r="BM4" s="74"/>
-      <c r="BN4" s="75"/>
-      <c r="BO4" s="73" t="str">
+      <c r="BI4" s="76"/>
+      <c r="BJ4" s="76"/>
+      <c r="BK4" s="76"/>
+      <c r="BL4" s="76"/>
+      <c r="BM4" s="76"/>
+      <c r="BN4" s="77"/>
+      <c r="BO4" s="75" t="str">
         <f>"Week "&amp;(BO6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 9</v>
       </c>
-      <c r="BP4" s="74"/>
-      <c r="BQ4" s="74"/>
-      <c r="BR4" s="74"/>
-      <c r="BS4" s="74"/>
-      <c r="BT4" s="74"/>
-      <c r="BU4" s="75"/>
-      <c r="BV4" s="73" t="str">
+      <c r="BP4" s="76"/>
+      <c r="BQ4" s="76"/>
+      <c r="BR4" s="76"/>
+      <c r="BS4" s="76"/>
+      <c r="BT4" s="76"/>
+      <c r="BU4" s="77"/>
+      <c r="BV4" s="75" t="str">
         <f>"Week "&amp;(BV6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 10</v>
       </c>
-      <c r="BW4" s="74"/>
-      <c r="BX4" s="74"/>
-      <c r="BY4" s="74"/>
-      <c r="BZ4" s="74"/>
-      <c r="CA4" s="74"/>
-      <c r="CB4" s="75"/>
+      <c r="BW4" s="76"/>
+      <c r="BX4" s="76"/>
+      <c r="BY4" s="76"/>
+      <c r="BZ4" s="76"/>
+      <c r="CA4" s="76"/>
+      <c r="CB4" s="77"/>
     </row>
     <row r="5" spans="1:80" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="45"/>
       <c r="B5" s="49" t="s">
         <v>10</v>
       </c>
-      <c r="C5" s="80" t="s">
+      <c r="C5" s="74" t="s">
         <v>14</v>
       </c>
-      <c r="D5" s="80"/>
-      <c r="E5" s="80"/>
+      <c r="D5" s="74"/>
+      <c r="E5" s="74"/>
       <c r="F5" s="48"/>
       <c r="G5" s="48"/>
       <c r="H5" s="48"/>
       <c r="I5" s="48"/>
       <c r="J5" s="13"/>
-      <c r="K5" s="76">
+      <c r="K5" s="79">
         <f>K6</f>
         <v>44662</v>
       </c>
-      <c r="L5" s="77"/>
-      <c r="M5" s="77"/>
-      <c r="N5" s="77"/>
-      <c r="O5" s="77"/>
-      <c r="P5" s="77"/>
-      <c r="Q5" s="78"/>
-      <c r="R5" s="76">
+      <c r="L5" s="80"/>
+      <c r="M5" s="80"/>
+      <c r="N5" s="80"/>
+      <c r="O5" s="80"/>
+      <c r="P5" s="80"/>
+      <c r="Q5" s="81"/>
+      <c r="R5" s="79">
         <f>R6</f>
         <v>44669</v>
       </c>
-      <c r="S5" s="77"/>
-      <c r="T5" s="77"/>
-      <c r="U5" s="77"/>
-      <c r="V5" s="77"/>
-      <c r="W5" s="77"/>
-      <c r="X5" s="78"/>
-      <c r="Y5" s="76">
+      <c r="S5" s="80"/>
+      <c r="T5" s="80"/>
+      <c r="U5" s="80"/>
+      <c r="V5" s="80"/>
+      <c r="W5" s="80"/>
+      <c r="X5" s="81"/>
+      <c r="Y5" s="79">
         <f>Y6</f>
         <v>44676</v>
       </c>
-      <c r="Z5" s="77"/>
-      <c r="AA5" s="77"/>
-      <c r="AB5" s="77"/>
-      <c r="AC5" s="77"/>
-      <c r="AD5" s="77"/>
-      <c r="AE5" s="78"/>
-      <c r="AF5" s="76">
+      <c r="Z5" s="80"/>
+      <c r="AA5" s="80"/>
+      <c r="AB5" s="80"/>
+      <c r="AC5" s="80"/>
+      <c r="AD5" s="80"/>
+      <c r="AE5" s="81"/>
+      <c r="AF5" s="79">
         <f>AF6</f>
         <v>44683</v>
       </c>
-      <c r="AG5" s="77"/>
-      <c r="AH5" s="77"/>
-      <c r="AI5" s="77"/>
-      <c r="AJ5" s="77"/>
-      <c r="AK5" s="77"/>
-      <c r="AL5" s="78"/>
-      <c r="AM5" s="76">
+      <c r="AG5" s="80"/>
+      <c r="AH5" s="80"/>
+      <c r="AI5" s="80"/>
+      <c r="AJ5" s="80"/>
+      <c r="AK5" s="80"/>
+      <c r="AL5" s="81"/>
+      <c r="AM5" s="79">
         <f>AM6</f>
         <v>44690</v>
       </c>
-      <c r="AN5" s="77"/>
-      <c r="AO5" s="77"/>
-      <c r="AP5" s="77"/>
-      <c r="AQ5" s="77"/>
-      <c r="AR5" s="77"/>
-      <c r="AS5" s="78"/>
-      <c r="AT5" s="76">
+      <c r="AN5" s="80"/>
+      <c r="AO5" s="80"/>
+      <c r="AP5" s="80"/>
+      <c r="AQ5" s="80"/>
+      <c r="AR5" s="80"/>
+      <c r="AS5" s="81"/>
+      <c r="AT5" s="79">
         <f>AT6</f>
         <v>44697</v>
       </c>
-      <c r="AU5" s="77"/>
-      <c r="AV5" s="77"/>
-      <c r="AW5" s="77"/>
-      <c r="AX5" s="77"/>
-      <c r="AY5" s="77"/>
-      <c r="AZ5" s="78"/>
-      <c r="BA5" s="76">
+      <c r="AU5" s="80"/>
+      <c r="AV5" s="80"/>
+      <c r="AW5" s="80"/>
+      <c r="AX5" s="80"/>
+      <c r="AY5" s="80"/>
+      <c r="AZ5" s="81"/>
+      <c r="BA5" s="79">
         <f>BA6</f>
         <v>44704</v>
       </c>
-      <c r="BB5" s="77"/>
-      <c r="BC5" s="77"/>
-      <c r="BD5" s="77"/>
-      <c r="BE5" s="77"/>
-      <c r="BF5" s="77"/>
-      <c r="BG5" s="78"/>
-      <c r="BH5" s="76">
+      <c r="BB5" s="80"/>
+      <c r="BC5" s="80"/>
+      <c r="BD5" s="80"/>
+      <c r="BE5" s="80"/>
+      <c r="BF5" s="80"/>
+      <c r="BG5" s="81"/>
+      <c r="BH5" s="79">
         <f>BH6</f>
         <v>44711</v>
       </c>
-      <c r="BI5" s="77"/>
-      <c r="BJ5" s="77"/>
-      <c r="BK5" s="77"/>
-      <c r="BL5" s="77"/>
-      <c r="BM5" s="77"/>
-      <c r="BN5" s="78"/>
-      <c r="BO5" s="76">
+      <c r="BI5" s="80"/>
+      <c r="BJ5" s="80"/>
+      <c r="BK5" s="80"/>
+      <c r="BL5" s="80"/>
+      <c r="BM5" s="80"/>
+      <c r="BN5" s="81"/>
+      <c r="BO5" s="79">
         <f>BO6</f>
         <v>44718</v>
       </c>
-      <c r="BP5" s="77"/>
-      <c r="BQ5" s="77"/>
-      <c r="BR5" s="77"/>
-      <c r="BS5" s="77"/>
-      <c r="BT5" s="77"/>
-      <c r="BU5" s="78"/>
-      <c r="BV5" s="76">
+      <c r="BP5" s="80"/>
+      <c r="BQ5" s="80"/>
+      <c r="BR5" s="80"/>
+      <c r="BS5" s="80"/>
+      <c r="BT5" s="80"/>
+      <c r="BU5" s="81"/>
+      <c r="BV5" s="79">
         <f>BV6</f>
         <v>44725</v>
       </c>
-      <c r="BW5" s="77"/>
-      <c r="BX5" s="77"/>
-      <c r="BY5" s="77"/>
-      <c r="BZ5" s="77"/>
-      <c r="CA5" s="77"/>
-      <c r="CB5" s="78"/>
+      <c r="BW5" s="80"/>
+      <c r="BX5" s="80"/>
+      <c r="BY5" s="80"/>
+      <c r="BZ5" s="80"/>
+      <c r="CA5" s="80"/>
+      <c r="CB5" s="81"/>
     </row>
     <row r="6" spans="1:80" x14ac:dyDescent="0.3">
       <c r="A6" s="12"/>
@@ -2707,7 +2725,7 @@
         <v>44731</v>
       </c>
     </row>
-    <row r="7" spans="1:80" s="59" customFormat="1" ht="23.6" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:80" s="59" customFormat="1" ht="31.3" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A7" s="51" t="s">
         <v>0</v>
       </c>
@@ -3033,7 +3051,7 @@
       <c r="G8" s="34"/>
       <c r="H8" s="35"/>
       <c r="I8" s="36" t="str">
-        <f t="shared" ref="I8:I30" si="20">IF(OR(F8=0,E8=0)," - ",NETWORKDAYS(E8,F8))</f>
+        <f t="shared" ref="I8:I31" si="20">IF(OR(F8=0,E8=0)," - ",NETWORKDAYS(E8,F8))</f>
         <v xml:space="preserve"> - </v>
       </c>
       <c r="J8" s="39"/>
@@ -3124,8 +3142,8 @@
         <v>44670</v>
       </c>
       <c r="G9" s="25">
-        <f>_xlfn.DAYS(F9,E9)</f>
-        <v>9</v>
+        <f>_xlfn.DAYS(F9,E9)+1</f>
+        <v>10</v>
       </c>
       <c r="H9" s="26">
         <v>1</v>
@@ -3315,8 +3333,8 @@
         <v>44673</v>
       </c>
       <c r="G11" s="25">
-        <f>_xlfn.DAYS(F11,E11)</f>
-        <v>3</v>
+        <f>_xlfn.DAYS(F11,E11)+1</f>
+        <v>4</v>
       </c>
       <c r="H11" s="26">
         <v>1</v>
@@ -3413,8 +3431,8 @@
         <v>44676</v>
       </c>
       <c r="G12" s="25">
-        <f>_xlfn.DAYS(F12,E12)</f>
-        <v>3</v>
+        <f t="shared" ref="G12:G17" si="23">_xlfn.DAYS(F12,E12)+1</f>
+        <v>4</v>
       </c>
       <c r="H12" s="26">
         <v>1</v>
@@ -3511,8 +3529,8 @@
         <v>44680</v>
       </c>
       <c r="G13" s="25">
-        <f t="shared" ref="G13:G17" si="23">_xlfn.DAYS(F13,E13)</f>
-        <v>4</v>
+        <f t="shared" si="23"/>
+        <v>5</v>
       </c>
       <c r="H13" s="26">
         <v>1</v>
@@ -3610,7 +3628,7 @@
       </c>
       <c r="G14" s="25">
         <f t="shared" si="23"/>
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="H14" s="26">
         <v>1</v>
@@ -3708,7 +3726,7 @@
       </c>
       <c r="G15" s="25">
         <f t="shared" si="23"/>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="H15" s="26">
         <v>1</v>
@@ -3806,7 +3824,7 @@
       </c>
       <c r="G16" s="25">
         <f t="shared" si="23"/>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="H16" s="26">
         <v>1</v>
@@ -3904,7 +3922,7 @@
       </c>
       <c r="G17" s="25">
         <f t="shared" si="23"/>
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="H17" s="26">
         <v>1</v>
@@ -3996,7 +4014,7 @@
       <c r="D18" s="19"/>
       <c r="E18" s="70"/>
       <c r="F18" s="70" t="str">
-        <f t="shared" ref="F18:F29" si="24">IF(ISBLANK(E18)," - ",IF(G18=0,E18,E18+G18-1))</f>
+        <f t="shared" ref="F18:F30" si="24">IF(ISBLANK(E18)," - ",IF(G18=0,E18,E18+G18-1))</f>
         <v xml:space="preserve"> - </v>
       </c>
       <c r="G18" s="20"/>
@@ -4079,7 +4097,7 @@
     </row>
     <row r="19" spans="1:80" s="24" customFormat="1" ht="115.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="23" t="str">
-        <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",1))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",2))-FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1)))+1)))</f>
+        <f t="shared" ref="A19:A26" si="25">IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",1))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",2))-FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1)))+1)))</f>
         <v>3.1</v>
       </c>
       <c r="B19" s="61" t="s">
@@ -4093,8 +4111,8 @@
         <v>44710</v>
       </c>
       <c r="G19" s="25">
-        <f>_xlfn.DAYS(F19,E19)</f>
-        <v>7</v>
+        <f>_xlfn.DAYS(F19,E19)+1</f>
+        <v>8</v>
       </c>
       <c r="H19" s="26">
         <v>1</v>
@@ -4177,7 +4195,7 @@
     </row>
     <row r="20" spans="1:80" s="24" customFormat="1" ht="147.44999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="23" t="str">
-        <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",1))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",2))-FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1)))+1)))</f>
+        <f t="shared" si="25"/>
         <v>3.2</v>
       </c>
       <c r="B20" s="61" t="s">
@@ -4191,8 +4209,8 @@
         <v>44715</v>
       </c>
       <c r="G20" s="25">
-        <f t="shared" ref="G20:G25" si="25">_xlfn.DAYS(F20,E20)</f>
-        <v>5</v>
+        <f t="shared" ref="G20:G26" si="26">_xlfn.DAYS(F20,E20)+1</f>
+        <v>6</v>
       </c>
       <c r="H20" s="26">
         <v>1</v>
@@ -4275,7 +4293,7 @@
     </row>
     <row r="21" spans="1:80" s="24" customFormat="1" ht="115.75" x14ac:dyDescent="0.3">
       <c r="A21" s="23" t="str">
-        <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",1))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",2))-FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1)))+1)))</f>
+        <f t="shared" si="25"/>
         <v>3.3</v>
       </c>
       <c r="B21" s="61" t="s">
@@ -4289,8 +4307,8 @@
         <v>44720</v>
       </c>
       <c r="G21" s="25">
-        <f t="shared" si="25"/>
-        <v>5</v>
+        <f t="shared" si="26"/>
+        <v>6</v>
       </c>
       <c r="H21" s="26">
         <v>1</v>
@@ -4373,7 +4391,7 @@
     </row>
     <row r="22" spans="1:80" s="24" customFormat="1" ht="188.15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="23" t="str">
-        <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",1))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",2))-FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1)))+1)))</f>
+        <f t="shared" si="25"/>
         <v>3.4</v>
       </c>
       <c r="B22" s="61" t="s">
@@ -4387,8 +4405,8 @@
         <v>44724</v>
       </c>
       <c r="G22" s="25">
-        <f t="shared" si="25"/>
-        <v>4</v>
+        <f t="shared" si="26"/>
+        <v>5</v>
       </c>
       <c r="H22" s="26">
         <v>1</v>
@@ -4471,7 +4489,7 @@
     </row>
     <row r="23" spans="1:80" s="24" customFormat="1" ht="109.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" s="23" t="str">
-        <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",1))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",2))-FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1)))+1)))</f>
+        <f t="shared" si="25"/>
         <v>3.5</v>
       </c>
       <c r="B23" s="61" t="s">
@@ -4485,14 +4503,14 @@
         <v>44728</v>
       </c>
       <c r="G23" s="25">
-        <f t="shared" si="25"/>
-        <v>4</v>
+        <f t="shared" si="26"/>
+        <v>5</v>
       </c>
       <c r="H23" s="26">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I23" s="27">
-        <f t="shared" ref="I23:I24" si="26">IF(OR(F23=0,E23=0)," - ",NETWORKDAYS(E23,F23))</f>
+        <f t="shared" ref="I23:I24" si="27">IF(OR(F23=0,E23=0)," - ",NETWORKDAYS(E23,F23))</f>
         <v>4</v>
       </c>
       <c r="J23" s="40"/>
@@ -4569,7 +4587,7 @@
     </row>
     <row r="24" spans="1:80" s="24" customFormat="1" ht="104.15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" s="23" t="str">
-        <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",1))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",2))-FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1)))+1)))</f>
+        <f t="shared" si="25"/>
         <v>3.6</v>
       </c>
       <c r="B24" s="61" t="s">
@@ -4583,14 +4601,14 @@
         <v>44731</v>
       </c>
       <c r="G24" s="25">
-        <f t="shared" si="25"/>
-        <v>3</v>
+        <f t="shared" si="26"/>
+        <v>4</v>
       </c>
       <c r="H24" s="26">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="I24" s="27">
-        <f t="shared" si="26"/>
+        <f t="shared" si="27"/>
         <v>2</v>
       </c>
       <c r="J24" s="40"/>
@@ -4667,7 +4685,7 @@
     </row>
     <row r="25" spans="1:80" s="24" customFormat="1" ht="85.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" s="23" t="str">
-        <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",1))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",2))-FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1)))+1)))</f>
+        <f t="shared" si="25"/>
         <v>3.7</v>
       </c>
       <c r="B25" s="61" t="s">
@@ -4681,14 +4699,14 @@
         <v>44733</v>
       </c>
       <c r="G25" s="25">
-        <f t="shared" si="25"/>
-        <v>2</v>
+        <f t="shared" si="26"/>
+        <v>3</v>
       </c>
       <c r="H25" s="26">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="I25" s="27">
-        <f t="shared" ref="I25" si="27">IF(OR(F25=0,E25=0)," - ",NETWORKDAYS(E25,F25))</f>
+        <f t="shared" ref="I25:I26" si="28">IF(OR(F25=0,E25=0)," - ",NETWORKDAYS(E25,F25))</f>
         <v>2</v>
       </c>
       <c r="J25" s="40"/>
@@ -4763,221 +4781,221 @@
       <c r="CA25" s="43"/>
       <c r="CB25" s="43"/>
     </row>
-    <row r="26" spans="1:80" s="18" customFormat="1" ht="17.600000000000001" x14ac:dyDescent="0.3">
-      <c r="A26" s="16" t="str">
+    <row r="26" spans="1:80" s="24" customFormat="1" ht="123" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="23" t="str">
+        <f t="shared" si="25"/>
+        <v>3.8</v>
+      </c>
+      <c r="B26" s="61" t="s">
+        <v>37</v>
+      </c>
+      <c r="D26" s="82"/>
+      <c r="E26" s="83">
+        <v>44733</v>
+      </c>
+      <c r="F26" s="84">
+        <v>44734</v>
+      </c>
+      <c r="G26" s="25">
+        <f t="shared" si="26"/>
+        <v>2</v>
+      </c>
+      <c r="H26" s="26">
+        <v>1</v>
+      </c>
+      <c r="I26" s="85">
+        <f t="shared" si="28"/>
+        <v>2</v>
+      </c>
+      <c r="J26" s="86"/>
+      <c r="K26" s="43"/>
+      <c r="L26" s="43"/>
+      <c r="M26" s="43"/>
+      <c r="N26" s="43"/>
+      <c r="O26" s="43"/>
+      <c r="P26" s="43"/>
+      <c r="Q26" s="43"/>
+      <c r="R26" s="43"/>
+      <c r="S26" s="43"/>
+      <c r="T26" s="43"/>
+      <c r="U26" s="43"/>
+      <c r="V26" s="43"/>
+      <c r="W26" s="43"/>
+      <c r="X26" s="43"/>
+      <c r="Y26" s="43"/>
+      <c r="Z26" s="43"/>
+      <c r="AA26" s="43"/>
+      <c r="AB26" s="43"/>
+      <c r="AC26" s="43"/>
+      <c r="AD26" s="43"/>
+      <c r="AE26" s="43"/>
+      <c r="AF26" s="43"/>
+      <c r="AG26" s="43"/>
+      <c r="AH26" s="43"/>
+      <c r="AI26" s="43"/>
+      <c r="AJ26" s="43"/>
+      <c r="AK26" s="43"/>
+      <c r="AL26" s="43"/>
+      <c r="AM26" s="43"/>
+      <c r="AN26" s="43"/>
+      <c r="AO26" s="43"/>
+      <c r="AP26" s="43"/>
+      <c r="AQ26" s="43"/>
+      <c r="AR26" s="43"/>
+      <c r="AS26" s="43"/>
+      <c r="AT26" s="43"/>
+      <c r="AU26" s="43"/>
+      <c r="AV26" s="43"/>
+      <c r="AW26" s="43"/>
+      <c r="AX26" s="43"/>
+      <c r="AY26" s="43"/>
+      <c r="AZ26" s="43"/>
+      <c r="BA26" s="43"/>
+      <c r="BB26" s="43"/>
+      <c r="BC26" s="43"/>
+      <c r="BD26" s="43"/>
+      <c r="BE26" s="43"/>
+      <c r="BF26" s="43"/>
+      <c r="BG26" s="43"/>
+      <c r="BH26" s="43"/>
+      <c r="BI26" s="43"/>
+      <c r="BJ26" s="43"/>
+      <c r="BK26" s="43"/>
+      <c r="BL26" s="43"/>
+      <c r="BM26" s="43"/>
+      <c r="BN26" s="43"/>
+      <c r="BO26" s="43"/>
+      <c r="BP26" s="43"/>
+      <c r="BQ26" s="43"/>
+      <c r="BR26" s="43"/>
+      <c r="BS26" s="43"/>
+      <c r="BT26" s="43"/>
+      <c r="BU26" s="43"/>
+      <c r="BV26" s="43"/>
+      <c r="BW26" s="43"/>
+      <c r="BX26" s="43"/>
+      <c r="BY26" s="43"/>
+      <c r="BZ26" s="43"/>
+      <c r="CA26" s="43"/>
+      <c r="CB26" s="43"/>
+    </row>
+    <row r="27" spans="1:80" s="18" customFormat="1" ht="17.600000000000001" x14ac:dyDescent="0.3">
+      <c r="A27" s="16" t="str">
         <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),TEXT(VALUE(prevWBS)+1,"#"),TEXT(VALUE(LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1))+1,"#")))</f>
         <v>4</v>
       </c>
-      <c r="B26" s="17" t="s">
+      <c r="B27" s="17" t="s">
         <v>27</v>
       </c>
-      <c r="D26" s="19"/>
-      <c r="E26" s="70"/>
-      <c r="F26" s="70" t="str">
+      <c r="D27" s="19"/>
+      <c r="E27" s="70"/>
+      <c r="F27" s="70" t="str">
         <f t="shared" si="24"/>
         <v xml:space="preserve"> - </v>
       </c>
-      <c r="G26" s="20"/>
-      <c r="H26" s="21"/>
-      <c r="I26" s="22" t="str">
+      <c r="G27" s="20"/>
+      <c r="H27" s="21"/>
+      <c r="I27" s="22" t="str">
         <f t="shared" si="20"/>
         <v xml:space="preserve"> - </v>
       </c>
-      <c r="J26" s="41"/>
-      <c r="K26" s="44"/>
-      <c r="L26" s="44"/>
-      <c r="M26" s="44"/>
-      <c r="N26" s="44"/>
-      <c r="O26" s="44"/>
-      <c r="P26" s="44"/>
-      <c r="Q26" s="44"/>
-      <c r="R26" s="44"/>
-      <c r="S26" s="44"/>
-      <c r="T26" s="44"/>
-      <c r="U26" s="44"/>
-      <c r="V26" s="44"/>
-      <c r="W26" s="44"/>
-      <c r="X26" s="44"/>
-      <c r="Y26" s="44"/>
-      <c r="Z26" s="44"/>
-      <c r="AA26" s="44"/>
-      <c r="AB26" s="44"/>
-      <c r="AC26" s="44"/>
-      <c r="AD26" s="44"/>
-      <c r="AE26" s="44"/>
-      <c r="AF26" s="44"/>
-      <c r="AG26" s="44"/>
-      <c r="AH26" s="44"/>
-      <c r="AI26" s="44"/>
-      <c r="AJ26" s="44"/>
-      <c r="AK26" s="44"/>
-      <c r="AL26" s="44"/>
-      <c r="AM26" s="44"/>
-      <c r="AN26" s="44"/>
-      <c r="AO26" s="44"/>
-      <c r="AP26" s="44"/>
-      <c r="AQ26" s="44"/>
-      <c r="AR26" s="44"/>
-      <c r="AS26" s="44"/>
-      <c r="AT26" s="44"/>
-      <c r="AU26" s="44"/>
-      <c r="AV26" s="44"/>
-      <c r="AW26" s="44"/>
-      <c r="AX26" s="44"/>
-      <c r="AY26" s="44"/>
-      <c r="AZ26" s="44"/>
-      <c r="BA26" s="44"/>
-      <c r="BB26" s="44"/>
-      <c r="BC26" s="44"/>
-      <c r="BD26" s="44"/>
-      <c r="BE26" s="44"/>
-      <c r="BF26" s="44"/>
-      <c r="BG26" s="44"/>
-      <c r="BH26" s="44"/>
-      <c r="BI26" s="44"/>
-      <c r="BJ26" s="44"/>
-      <c r="BK26" s="44"/>
-      <c r="BL26" s="44"/>
-      <c r="BM26" s="44"/>
-      <c r="BN26" s="44"/>
-      <c r="BO26" s="44"/>
-      <c r="BP26" s="44"/>
-      <c r="BQ26" s="44"/>
-      <c r="BR26" s="44"/>
-      <c r="BS26" s="44"/>
-      <c r="BT26" s="44"/>
-      <c r="BU26" s="44"/>
-      <c r="BV26" s="44"/>
-      <c r="BW26" s="44"/>
-      <c r="BX26" s="44"/>
-      <c r="BY26" s="44"/>
-      <c r="BZ26" s="44"/>
-      <c r="CA26" s="44"/>
-      <c r="CB26" s="44"/>
+      <c r="J27" s="41"/>
+      <c r="K27" s="44"/>
+      <c r="L27" s="44"/>
+      <c r="M27" s="44"/>
+      <c r="N27" s="44"/>
+      <c r="O27" s="44"/>
+      <c r="P27" s="44"/>
+      <c r="Q27" s="44"/>
+      <c r="R27" s="44"/>
+      <c r="S27" s="44"/>
+      <c r="T27" s="44"/>
+      <c r="U27" s="44"/>
+      <c r="V27" s="44"/>
+      <c r="W27" s="44"/>
+      <c r="X27" s="44"/>
+      <c r="Y27" s="44"/>
+      <c r="Z27" s="44"/>
+      <c r="AA27" s="44"/>
+      <c r="AB27" s="44"/>
+      <c r="AC27" s="44"/>
+      <c r="AD27" s="44"/>
+      <c r="AE27" s="44"/>
+      <c r="AF27" s="44"/>
+      <c r="AG27" s="44"/>
+      <c r="AH27" s="44"/>
+      <c r="AI27" s="44"/>
+      <c r="AJ27" s="44"/>
+      <c r="AK27" s="44"/>
+      <c r="AL27" s="44"/>
+      <c r="AM27" s="44"/>
+      <c r="AN27" s="44"/>
+      <c r="AO27" s="44"/>
+      <c r="AP27" s="44"/>
+      <c r="AQ27" s="44"/>
+      <c r="AR27" s="44"/>
+      <c r="AS27" s="44"/>
+      <c r="AT27" s="44"/>
+      <c r="AU27" s="44"/>
+      <c r="AV27" s="44"/>
+      <c r="AW27" s="44"/>
+      <c r="AX27" s="44"/>
+      <c r="AY27" s="44"/>
+      <c r="AZ27" s="44"/>
+      <c r="BA27" s="44"/>
+      <c r="BB27" s="44"/>
+      <c r="BC27" s="44"/>
+      <c r="BD27" s="44"/>
+      <c r="BE27" s="44"/>
+      <c r="BF27" s="44"/>
+      <c r="BG27" s="44"/>
+      <c r="BH27" s="44"/>
+      <c r="BI27" s="44"/>
+      <c r="BJ27" s="44"/>
+      <c r="BK27" s="44"/>
+      <c r="BL27" s="44"/>
+      <c r="BM27" s="44"/>
+      <c r="BN27" s="44"/>
+      <c r="BO27" s="44"/>
+      <c r="BP27" s="44"/>
+      <c r="BQ27" s="44"/>
+      <c r="BR27" s="44"/>
+      <c r="BS27" s="44"/>
+      <c r="BT27" s="44"/>
+      <c r="BU27" s="44"/>
+      <c r="BV27" s="44"/>
+      <c r="BW27" s="44"/>
+      <c r="BX27" s="44"/>
+      <c r="BY27" s="44"/>
+      <c r="BZ27" s="44"/>
+      <c r="CA27" s="44"/>
+      <c r="CB27" s="44"/>
     </row>
-    <row r="27" spans="1:80" s="24" customFormat="1" ht="70.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="23" t="str">
+    <row r="28" spans="1:80" s="24" customFormat="1" ht="70.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A28" s="23" t="str">
         <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",1))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",2))-FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1)))+1)))</f>
         <v>4.1</v>
       </c>
-      <c r="B27" s="61" t="s">
+      <c r="B28" s="61" t="s">
         <v>36</v>
       </c>
-      <c r="D27" s="62"/>
-      <c r="E27" s="68">
+      <c r="D28" s="62"/>
+      <c r="E28" s="68">
         <v>44691</v>
       </c>
-      <c r="F27" s="71">
+      <c r="F28" s="71">
         <v>44733</v>
       </c>
-      <c r="G27" s="25">
-        <f>_xlfn.DAYS(F27,E27)</f>
-        <v>42</v>
-      </c>
-      <c r="H27" s="26">
+      <c r="G28" s="25">
+        <f>_xlfn.DAYS(F28,E28)+1</f>
+        <v>43</v>
+      </c>
+      <c r="H28" s="26">
         <v>1</v>
       </c>
-      <c r="I27" s="27">
+      <c r="I28" s="27">
         <f t="shared" si="20"/>
         <v>31</v>
-      </c>
-      <c r="J27" s="40"/>
-      <c r="K27" s="43"/>
-      <c r="L27" s="43"/>
-      <c r="M27" s="43"/>
-      <c r="N27" s="43"/>
-      <c r="O27" s="43"/>
-      <c r="P27" s="43"/>
-      <c r="Q27" s="43"/>
-      <c r="R27" s="43"/>
-      <c r="S27" s="43"/>
-      <c r="T27" s="43"/>
-      <c r="U27" s="43"/>
-      <c r="V27" s="43"/>
-      <c r="W27" s="43"/>
-      <c r="X27" s="43"/>
-      <c r="Y27" s="43"/>
-      <c r="Z27" s="43"/>
-      <c r="AA27" s="43"/>
-      <c r="AB27" s="43"/>
-      <c r="AC27" s="43"/>
-      <c r="AD27" s="43"/>
-      <c r="AE27" s="43"/>
-      <c r="AF27" s="43"/>
-      <c r="AG27" s="43"/>
-      <c r="AH27" s="43"/>
-      <c r="AI27" s="43"/>
-      <c r="AJ27" s="43"/>
-      <c r="AK27" s="43"/>
-      <c r="AL27" s="43"/>
-      <c r="AM27" s="43"/>
-      <c r="AN27" s="43"/>
-      <c r="AO27" s="43"/>
-      <c r="AP27" s="43"/>
-      <c r="AQ27" s="43"/>
-      <c r="AR27" s="43"/>
-      <c r="AS27" s="43"/>
-      <c r="AT27" s="43"/>
-      <c r="AU27" s="43"/>
-      <c r="AV27" s="43"/>
-      <c r="AW27" s="43"/>
-      <c r="AX27" s="43"/>
-      <c r="AY27" s="43"/>
-      <c r="AZ27" s="43"/>
-      <c r="BA27" s="43"/>
-      <c r="BB27" s="43"/>
-      <c r="BC27" s="43"/>
-      <c r="BD27" s="43"/>
-      <c r="BE27" s="43"/>
-      <c r="BF27" s="43"/>
-      <c r="BG27" s="43"/>
-      <c r="BH27" s="43"/>
-      <c r="BI27" s="43"/>
-      <c r="BJ27" s="43"/>
-      <c r="BK27" s="43"/>
-      <c r="BL27" s="43"/>
-      <c r="BM27" s="43"/>
-      <c r="BN27" s="43"/>
-      <c r="BO27" s="43"/>
-      <c r="BP27" s="43"/>
-      <c r="BQ27" s="43"/>
-      <c r="BR27" s="43"/>
-      <c r="BS27" s="43"/>
-      <c r="BT27" s="43"/>
-      <c r="BU27" s="43"/>
-      <c r="BV27" s="43"/>
-      <c r="BW27" s="43"/>
-      <c r="BX27" s="43"/>
-      <c r="BY27" s="43"/>
-      <c r="BZ27" s="43"/>
-      <c r="CA27" s="43"/>
-      <c r="CB27" s="43"/>
-    </row>
-    <row r="28" spans="1:80" s="24" customFormat="1" ht="37.299999999999997" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="23" t="str">
-        <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",1))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",2))-FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1)))+1)))</f>
-        <v>4.2</v>
-      </c>
-      <c r="B28" s="61" t="s">
-        <v>28</v>
-      </c>
-      <c r="D28" s="62"/>
-      <c r="E28" s="68">
-        <v>44733</v>
-      </c>
-      <c r="F28" s="71">
-        <v>44734</v>
-      </c>
-      <c r="G28" s="25">
-        <f>_xlfn.DAYS(F28,E28)</f>
-        <v>1</v>
-      </c>
-      <c r="H28" s="26">
-        <v>1</v>
-      </c>
-      <c r="I28" s="27">
-        <f t="shared" si="20"/>
-        <v>2</v>
       </c>
       <c r="J28" s="40"/>
       <c r="K28" s="43"/>
@@ -5051,221 +5069,221 @@
       <c r="CA28" s="43"/>
       <c r="CB28" s="43"/>
     </row>
-    <row r="29" spans="1:80" s="18" customFormat="1" ht="17.600000000000001" x14ac:dyDescent="0.3">
-      <c r="A29" s="16" t="str">
+    <row r="29" spans="1:80" s="24" customFormat="1" ht="37.299999999999997" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A29" s="23" t="str">
+        <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",1))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",2))-FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1)))+1)))</f>
+        <v>4.2</v>
+      </c>
+      <c r="B29" s="61" t="s">
+        <v>28</v>
+      </c>
+      <c r="D29" s="62"/>
+      <c r="E29" s="68">
+        <v>44733</v>
+      </c>
+      <c r="F29" s="71">
+        <v>44734</v>
+      </c>
+      <c r="G29" s="25">
+        <f>_xlfn.DAYS(F29,E29)+1</f>
+        <v>2</v>
+      </c>
+      <c r="H29" s="26">
+        <v>1</v>
+      </c>
+      <c r="I29" s="27">
+        <f t="shared" si="20"/>
+        <v>2</v>
+      </c>
+      <c r="J29" s="40"/>
+      <c r="K29" s="43"/>
+      <c r="L29" s="43"/>
+      <c r="M29" s="43"/>
+      <c r="N29" s="43"/>
+      <c r="O29" s="43"/>
+      <c r="P29" s="43"/>
+      <c r="Q29" s="43"/>
+      <c r="R29" s="43"/>
+      <c r="S29" s="43"/>
+      <c r="T29" s="43"/>
+      <c r="U29" s="43"/>
+      <c r="V29" s="43"/>
+      <c r="W29" s="43"/>
+      <c r="X29" s="43"/>
+      <c r="Y29" s="43"/>
+      <c r="Z29" s="43"/>
+      <c r="AA29" s="43"/>
+      <c r="AB29" s="43"/>
+      <c r="AC29" s="43"/>
+      <c r="AD29" s="43"/>
+      <c r="AE29" s="43"/>
+      <c r="AF29" s="43"/>
+      <c r="AG29" s="43"/>
+      <c r="AH29" s="43"/>
+      <c r="AI29" s="43"/>
+      <c r="AJ29" s="43"/>
+      <c r="AK29" s="43"/>
+      <c r="AL29" s="43"/>
+      <c r="AM29" s="43"/>
+      <c r="AN29" s="43"/>
+      <c r="AO29" s="43"/>
+      <c r="AP29" s="43"/>
+      <c r="AQ29" s="43"/>
+      <c r="AR29" s="43"/>
+      <c r="AS29" s="43"/>
+      <c r="AT29" s="43"/>
+      <c r="AU29" s="43"/>
+      <c r="AV29" s="43"/>
+      <c r="AW29" s="43"/>
+      <c r="AX29" s="43"/>
+      <c r="AY29" s="43"/>
+      <c r="AZ29" s="43"/>
+      <c r="BA29" s="43"/>
+      <c r="BB29" s="43"/>
+      <c r="BC29" s="43"/>
+      <c r="BD29" s="43"/>
+      <c r="BE29" s="43"/>
+      <c r="BF29" s="43"/>
+      <c r="BG29" s="43"/>
+      <c r="BH29" s="43"/>
+      <c r="BI29" s="43"/>
+      <c r="BJ29" s="43"/>
+      <c r="BK29" s="43"/>
+      <c r="BL29" s="43"/>
+      <c r="BM29" s="43"/>
+      <c r="BN29" s="43"/>
+      <c r="BO29" s="43"/>
+      <c r="BP29" s="43"/>
+      <c r="BQ29" s="43"/>
+      <c r="BR29" s="43"/>
+      <c r="BS29" s="43"/>
+      <c r="BT29" s="43"/>
+      <c r="BU29" s="43"/>
+      <c r="BV29" s="43"/>
+      <c r="BW29" s="43"/>
+      <c r="BX29" s="43"/>
+      <c r="BY29" s="43"/>
+      <c r="BZ29" s="43"/>
+      <c r="CA29" s="43"/>
+      <c r="CB29" s="43"/>
+    </row>
+    <row r="30" spans="1:80" s="18" customFormat="1" ht="17.600000000000001" x14ac:dyDescent="0.3">
+      <c r="A30" s="16" t="str">
         <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),TEXT(VALUE(prevWBS)+1,"#"),TEXT(VALUE(LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1))+1,"#")))</f>
         <v>5</v>
       </c>
-      <c r="B29" s="17" t="s">
+      <c r="B30" s="17" t="s">
         <v>11</v>
       </c>
-      <c r="D29" s="19"/>
-      <c r="E29" s="70"/>
-      <c r="F29" s="70" t="str">
+      <c r="D30" s="19"/>
+      <c r="E30" s="70"/>
+      <c r="F30" s="70" t="str">
         <f t="shared" si="24"/>
         <v xml:space="preserve"> - </v>
       </c>
-      <c r="G29" s="20"/>
-      <c r="H29" s="21"/>
-      <c r="I29" s="22" t="str">
+      <c r="G30" s="20"/>
+      <c r="H30" s="21"/>
+      <c r="I30" s="22" t="str">
         <f t="shared" si="20"/>
         <v xml:space="preserve"> - </v>
       </c>
-      <c r="J29" s="41"/>
-      <c r="K29" s="44"/>
-      <c r="L29" s="44"/>
-      <c r="M29" s="44"/>
-      <c r="N29" s="44"/>
-      <c r="O29" s="44"/>
-      <c r="P29" s="44"/>
-      <c r="Q29" s="44"/>
-      <c r="R29" s="44"/>
-      <c r="S29" s="44"/>
-      <c r="T29" s="44"/>
-      <c r="U29" s="44"/>
-      <c r="V29" s="44"/>
-      <c r="W29" s="44"/>
-      <c r="X29" s="44"/>
-      <c r="Y29" s="44"/>
-      <c r="Z29" s="44"/>
-      <c r="AA29" s="44"/>
-      <c r="AB29" s="44"/>
-      <c r="AC29" s="44"/>
-      <c r="AD29" s="44"/>
-      <c r="AE29" s="44"/>
-      <c r="AF29" s="44"/>
-      <c r="AG29" s="44"/>
-      <c r="AH29" s="44"/>
-      <c r="AI29" s="44"/>
-      <c r="AJ29" s="44"/>
-      <c r="AK29" s="44"/>
-      <c r="AL29" s="44"/>
-      <c r="AM29" s="44"/>
-      <c r="AN29" s="44"/>
-      <c r="AO29" s="44"/>
-      <c r="AP29" s="44"/>
-      <c r="AQ29" s="44"/>
-      <c r="AR29" s="44"/>
-      <c r="AS29" s="44"/>
-      <c r="AT29" s="44"/>
-      <c r="AU29" s="44"/>
-      <c r="AV29" s="44"/>
-      <c r="AW29" s="44"/>
-      <c r="AX29" s="44"/>
-      <c r="AY29" s="44"/>
-      <c r="AZ29" s="44"/>
-      <c r="BA29" s="44"/>
-      <c r="BB29" s="44"/>
-      <c r="BC29" s="44"/>
-      <c r="BD29" s="44"/>
-      <c r="BE29" s="44"/>
-      <c r="BF29" s="44"/>
-      <c r="BG29" s="44"/>
-      <c r="BH29" s="44"/>
-      <c r="BI29" s="44"/>
-      <c r="BJ29" s="44"/>
-      <c r="BK29" s="44"/>
-      <c r="BL29" s="44"/>
-      <c r="BM29" s="44"/>
-      <c r="BN29" s="44"/>
-      <c r="BO29" s="44"/>
-      <c r="BP29" s="44"/>
-      <c r="BQ29" s="44"/>
-      <c r="BR29" s="44"/>
-      <c r="BS29" s="44"/>
-      <c r="BT29" s="44"/>
-      <c r="BU29" s="44"/>
-      <c r="BV29" s="44"/>
-      <c r="BW29" s="44"/>
-      <c r="BX29" s="44"/>
-      <c r="BY29" s="44"/>
-      <c r="BZ29" s="44"/>
-      <c r="CA29" s="44"/>
-      <c r="CB29" s="44"/>
-    </row>
-    <row r="30" spans="1:80" s="24" customFormat="1" ht="17.600000000000001" x14ac:dyDescent="0.3">
-      <c r="A30" s="23" t="str">
-        <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",1))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",2))-FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1)))+1)))</f>
-        <v>5.1</v>
-      </c>
-      <c r="B30" s="61" t="s">
-        <v>24</v>
-      </c>
-      <c r="D30" s="62"/>
-      <c r="E30" s="68">
-        <v>44661</v>
-      </c>
-      <c r="F30" s="71">
-        <v>44733</v>
-      </c>
-      <c r="G30" s="25">
-        <f>_xlfn.DAYS(F30,E30)</f>
-        <v>72</v>
-      </c>
-      <c r="H30" s="26">
-        <v>1</v>
-      </c>
-      <c r="I30" s="27">
-        <f t="shared" si="20"/>
-        <v>52</v>
-      </c>
-      <c r="J30" s="40"/>
-      <c r="K30" s="43"/>
-      <c r="L30" s="43"/>
-      <c r="M30" s="43"/>
-      <c r="N30" s="43"/>
-      <c r="O30" s="43"/>
-      <c r="P30" s="43"/>
-      <c r="Q30" s="43"/>
-      <c r="R30" s="43"/>
-      <c r="S30" s="43"/>
-      <c r="T30" s="43"/>
-      <c r="U30" s="43"/>
-      <c r="V30" s="43"/>
-      <c r="W30" s="43"/>
-      <c r="X30" s="43"/>
-      <c r="Y30" s="43"/>
-      <c r="Z30" s="43"/>
-      <c r="AA30" s="43"/>
-      <c r="AB30" s="43"/>
-      <c r="AC30" s="43"/>
-      <c r="AD30" s="43"/>
-      <c r="AE30" s="43"/>
-      <c r="AF30" s="43"/>
-      <c r="AG30" s="43"/>
-      <c r="AH30" s="43"/>
-      <c r="AI30" s="43"/>
-      <c r="AJ30" s="43"/>
-      <c r="AK30" s="43"/>
-      <c r="AL30" s="43"/>
-      <c r="AM30" s="43"/>
-      <c r="AN30" s="43"/>
-      <c r="AO30" s="43"/>
-      <c r="AP30" s="43"/>
-      <c r="AQ30" s="43"/>
-      <c r="AR30" s="43"/>
-      <c r="AS30" s="43"/>
-      <c r="AT30" s="43"/>
-      <c r="AU30" s="43"/>
-      <c r="AV30" s="43"/>
-      <c r="AW30" s="43"/>
-      <c r="AX30" s="43"/>
-      <c r="AY30" s="43"/>
-      <c r="AZ30" s="43"/>
-      <c r="BA30" s="43"/>
-      <c r="BB30" s="43"/>
-      <c r="BC30" s="43"/>
-      <c r="BD30" s="43"/>
-      <c r="BE30" s="43"/>
-      <c r="BF30" s="43"/>
-      <c r="BG30" s="43"/>
-      <c r="BH30" s="43"/>
-      <c r="BI30" s="43"/>
-      <c r="BJ30" s="43"/>
-      <c r="BK30" s="43"/>
-      <c r="BL30" s="43"/>
-      <c r="BM30" s="43"/>
-      <c r="BN30" s="43"/>
-      <c r="BO30" s="43"/>
-      <c r="BP30" s="43"/>
-      <c r="BQ30" s="43"/>
-      <c r="BR30" s="43"/>
-      <c r="BS30" s="43"/>
-      <c r="BT30" s="43"/>
-      <c r="BU30" s="43"/>
-      <c r="BV30" s="43"/>
-      <c r="BW30" s="43"/>
-      <c r="BX30" s="43"/>
-      <c r="BY30" s="43"/>
-      <c r="BZ30" s="43"/>
-      <c r="CA30" s="43"/>
-      <c r="CB30" s="43"/>
+      <c r="J30" s="41"/>
+      <c r="K30" s="44"/>
+      <c r="L30" s="44"/>
+      <c r="M30" s="44"/>
+      <c r="N30" s="44"/>
+      <c r="O30" s="44"/>
+      <c r="P30" s="44"/>
+      <c r="Q30" s="44"/>
+      <c r="R30" s="44"/>
+      <c r="S30" s="44"/>
+      <c r="T30" s="44"/>
+      <c r="U30" s="44"/>
+      <c r="V30" s="44"/>
+      <c r="W30" s="44"/>
+      <c r="X30" s="44"/>
+      <c r="Y30" s="44"/>
+      <c r="Z30" s="44"/>
+      <c r="AA30" s="44"/>
+      <c r="AB30" s="44"/>
+      <c r="AC30" s="44"/>
+      <c r="AD30" s="44"/>
+      <c r="AE30" s="44"/>
+      <c r="AF30" s="44"/>
+      <c r="AG30" s="44"/>
+      <c r="AH30" s="44"/>
+      <c r="AI30" s="44"/>
+      <c r="AJ30" s="44"/>
+      <c r="AK30" s="44"/>
+      <c r="AL30" s="44"/>
+      <c r="AM30" s="44"/>
+      <c r="AN30" s="44"/>
+      <c r="AO30" s="44"/>
+      <c r="AP30" s="44"/>
+      <c r="AQ30" s="44"/>
+      <c r="AR30" s="44"/>
+      <c r="AS30" s="44"/>
+      <c r="AT30" s="44"/>
+      <c r="AU30" s="44"/>
+      <c r="AV30" s="44"/>
+      <c r="AW30" s="44"/>
+      <c r="AX30" s="44"/>
+      <c r="AY30" s="44"/>
+      <c r="AZ30" s="44"/>
+      <c r="BA30" s="44"/>
+      <c r="BB30" s="44"/>
+      <c r="BC30" s="44"/>
+      <c r="BD30" s="44"/>
+      <c r="BE30" s="44"/>
+      <c r="BF30" s="44"/>
+      <c r="BG30" s="44"/>
+      <c r="BH30" s="44"/>
+      <c r="BI30" s="44"/>
+      <c r="BJ30" s="44"/>
+      <c r="BK30" s="44"/>
+      <c r="BL30" s="44"/>
+      <c r="BM30" s="44"/>
+      <c r="BN30" s="44"/>
+      <c r="BO30" s="44"/>
+      <c r="BP30" s="44"/>
+      <c r="BQ30" s="44"/>
+      <c r="BR30" s="44"/>
+      <c r="BS30" s="44"/>
+      <c r="BT30" s="44"/>
+      <c r="BU30" s="44"/>
+      <c r="BV30" s="44"/>
+      <c r="BW30" s="44"/>
+      <c r="BX30" s="44"/>
+      <c r="BY30" s="44"/>
+      <c r="BZ30" s="44"/>
+      <c r="CA30" s="44"/>
+      <c r="CB30" s="44"/>
     </row>
     <row r="31" spans="1:80" s="24" customFormat="1" ht="17.600000000000001" x14ac:dyDescent="0.3">
       <c r="A31" s="23" t="str">
         <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",1))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",2))-FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1)))+1)))</f>
-        <v>5.2</v>
+        <v>5.1</v>
       </c>
       <c r="B31" s="61" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D31" s="62"/>
       <c r="E31" s="68">
-        <v>44729</v>
+        <v>44661</v>
       </c>
       <c r="F31" s="71">
         <v>44733</v>
       </c>
       <c r="G31" s="25">
-        <f>_xlfn.DAYS(F31,E31)</f>
-        <v>4</v>
+        <f>_xlfn.DAYS(F31,E31)+1</f>
+        <v>73</v>
       </c>
       <c r="H31" s="26">
         <v>1</v>
       </c>
       <c r="I31" s="27">
-        <f t="shared" ref="I31" si="28">IF(OR(F31=0,E31=0)," - ",NETWORKDAYS(E31,F31))</f>
-        <v>3</v>
+        <f t="shared" si="20"/>
+        <v>52</v>
       </c>
       <c r="J31" s="40"/>
       <c r="K31" s="43"/>
@@ -5339,18 +5357,107 @@
       <c r="CA31" s="43"/>
       <c r="CB31" s="43"/>
     </row>
+    <row r="32" spans="1:80" s="24" customFormat="1" ht="17.600000000000001" x14ac:dyDescent="0.3">
+      <c r="A32" s="23" t="str">
+        <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",1))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",2))-FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1)))+1)))</f>
+        <v>5.2</v>
+      </c>
+      <c r="B32" s="61" t="s">
+        <v>25</v>
+      </c>
+      <c r="D32" s="62"/>
+      <c r="E32" s="68">
+        <v>44729</v>
+      </c>
+      <c r="F32" s="71">
+        <v>44733</v>
+      </c>
+      <c r="G32" s="25">
+        <f>_xlfn.DAYS(F32,E32)+1</f>
+        <v>5</v>
+      </c>
+      <c r="H32" s="26">
+        <v>1</v>
+      </c>
+      <c r="I32" s="27">
+        <f t="shared" ref="I32" si="29">IF(OR(F32=0,E32=0)," - ",NETWORKDAYS(E32,F32))</f>
+        <v>3</v>
+      </c>
+      <c r="J32" s="40"/>
+      <c r="K32" s="43"/>
+      <c r="L32" s="43"/>
+      <c r="M32" s="43"/>
+      <c r="N32" s="43"/>
+      <c r="O32" s="43"/>
+      <c r="P32" s="43"/>
+      <c r="Q32" s="43"/>
+      <c r="R32" s="43"/>
+      <c r="S32" s="43"/>
+      <c r="T32" s="43"/>
+      <c r="U32" s="43"/>
+      <c r="V32" s="43"/>
+      <c r="W32" s="43"/>
+      <c r="X32" s="43"/>
+      <c r="Y32" s="43"/>
+      <c r="Z32" s="43"/>
+      <c r="AA32" s="43"/>
+      <c r="AB32" s="43"/>
+      <c r="AC32" s="43"/>
+      <c r="AD32" s="43"/>
+      <c r="AE32" s="43"/>
+      <c r="AF32" s="43"/>
+      <c r="AG32" s="43"/>
+      <c r="AH32" s="43"/>
+      <c r="AI32" s="43"/>
+      <c r="AJ32" s="43"/>
+      <c r="AK32" s="43"/>
+      <c r="AL32" s="43"/>
+      <c r="AM32" s="43"/>
+      <c r="AN32" s="43"/>
+      <c r="AO32" s="43"/>
+      <c r="AP32" s="43"/>
+      <c r="AQ32" s="43"/>
+      <c r="AR32" s="43"/>
+      <c r="AS32" s="43"/>
+      <c r="AT32" s="43"/>
+      <c r="AU32" s="43"/>
+      <c r="AV32" s="43"/>
+      <c r="AW32" s="43"/>
+      <c r="AX32" s="43"/>
+      <c r="AY32" s="43"/>
+      <c r="AZ32" s="43"/>
+      <c r="BA32" s="43"/>
+      <c r="BB32" s="43"/>
+      <c r="BC32" s="43"/>
+      <c r="BD32" s="43"/>
+      <c r="BE32" s="43"/>
+      <c r="BF32" s="43"/>
+      <c r="BG32" s="43"/>
+      <c r="BH32" s="43"/>
+      <c r="BI32" s="43"/>
+      <c r="BJ32" s="43"/>
+      <c r="BK32" s="43"/>
+      <c r="BL32" s="43"/>
+      <c r="BM32" s="43"/>
+      <c r="BN32" s="43"/>
+      <c r="BO32" s="43"/>
+      <c r="BP32" s="43"/>
+      <c r="BQ32" s="43"/>
+      <c r="BR32" s="43"/>
+      <c r="BS32" s="43"/>
+      <c r="BT32" s="43"/>
+      <c r="BU32" s="43"/>
+      <c r="BV32" s="43"/>
+      <c r="BW32" s="43"/>
+      <c r="BX32" s="43"/>
+      <c r="BY32" s="43"/>
+      <c r="BZ32" s="43"/>
+      <c r="CA32" s="43"/>
+      <c r="CB32" s="43"/>
+    </row>
   </sheetData>
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertRows="0" deleteRows="0"/>
   <mergeCells count="23">
-    <mergeCell ref="K1:AE1"/>
-    <mergeCell ref="C5:E5"/>
-    <mergeCell ref="R4:X4"/>
-    <mergeCell ref="K4:Q4"/>
-    <mergeCell ref="C4:E4"/>
-    <mergeCell ref="R5:X5"/>
-    <mergeCell ref="K5:Q5"/>
-    <mergeCell ref="Y4:AE4"/>
-    <mergeCell ref="Y5:AE5"/>
     <mergeCell ref="BO4:BU4"/>
     <mergeCell ref="BO5:BU5"/>
     <mergeCell ref="BV4:CB4"/>
@@ -5365,9 +5472,18 @@
     <mergeCell ref="AM4:AS4"/>
     <mergeCell ref="BA4:BG4"/>
     <mergeCell ref="BA5:BG5"/>
+    <mergeCell ref="K1:AE1"/>
+    <mergeCell ref="C5:E5"/>
+    <mergeCell ref="R4:X4"/>
+    <mergeCell ref="K4:Q4"/>
+    <mergeCell ref="C4:E4"/>
+    <mergeCell ref="R5:X5"/>
+    <mergeCell ref="K5:Q5"/>
+    <mergeCell ref="Y4:AE4"/>
+    <mergeCell ref="Y5:AE5"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
-  <conditionalFormatting sqref="H8:H9 H17:H31 H11:H14">
+  <conditionalFormatting sqref="H8:H9 H11:H14 H17:H32">
     <cfRule type="dataBar" priority="10">
       <dataBar>
         <cfvo type="num" val="0"/>
@@ -5386,7 +5502,7 @@
       <formula>K$6=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K8:CB31">
+  <conditionalFormatting sqref="K8:CB32">
     <cfRule type="expression" dxfId="4" priority="56">
       <formula>AND($E8&lt;=K$6,ROUNDDOWN(($F8-$E8+1)*$H8,0)+$E8-1&gt;=K$6)</formula>
     </cfRule>
@@ -5394,7 +5510,7 @@
       <formula>AND(NOT(ISBLANK($E8)),$E8&lt;=K$6,$F8&gt;=K$6)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K6:CB9 K17:CB31 K11:CB14">
+  <conditionalFormatting sqref="K6:CB9 K17:CB32 K11:CB14">
     <cfRule type="expression" dxfId="2" priority="16">
       <formula>K$6=TODAY()</formula>
     </cfRule>
@@ -5444,8 +5560,8 @@
   <pageSetup paperSize="8" scale="96" fitToHeight="0" orientation="landscape" r:id="rId1"/>
   <headerFooter alignWithMargins="0"/>
   <ignoredErrors>
-    <ignoredError sqref="H9 E18 E26 E29 G18:H18 G26:H26 G29:H29" unlockedFormula="1"/>
-    <ignoredError sqref="A29 A26 A18" formula="1"/>
+    <ignoredError sqref="H9 E18 E27 E30 G18:H18 G27:H27 G30:H30" unlockedFormula="1"/>
+    <ignoredError sqref="A30 A27 A18" formula="1"/>
   </ignoredErrors>
   <drawing r:id="rId2"/>
   <legacyDrawing r:id="rId3"/>
@@ -5493,7 +5609,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>H8:H9 H17:H31 H11:H14</xm:sqref>
+          <xm:sqref>H8:H9 H11:H14 H17:H32</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{39040515-52F3-4094-B202-ACD1080964D7}">

</xml_diff>